<commit_message>
Se actualiza el proyecto para que ahora funcione con el nuevo jar ya que se hizo una reestructuracion de los paquetes
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/SVE_TRN0385_Autenticacion.xlsx
+++ b/src/test/resources/datadriven/SVE_TRN0385_Autenticacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qv-3795\eclipse-workspace\pruebajarlogin\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00486D6-EA95-42AE-8224-5CB120019549}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D05388-E01B-403B-8E1D-24AD7176C2DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,10 +166,10 @@
     <t>qqqqqqqq</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>usuariotest</t>
+    <t>800270811</t>
+  </si>
+  <si>
+    <t>autouser1994</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>